<commit_message>
Add compiled results with metadata
</commit_message>
<xml_diff>
--- a/Freq_all.xlsx
+++ b/Freq_all.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alandler/OneDrive - Massachusetts Institute of Technology/15.053/GIT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod-my.sharepoint.com/personal/alandler_mit_edu/Documents/15.053/GIT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E703741-87A9-3C46-BD7E-4FBA9A575002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{5E703741-87A9-3C46-BD7E-4FBA9A575002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{901C27D9-9703-B24E-9511-281C2307C223}"/>
   <bookViews>
-    <workbookView xWindow="20000" yWindow="460" windowWidth="26440" windowHeight="15440" xr2:uid="{97C33AB7-0840-E244-BC44-7C9BE2576C51}"/>
+    <workbookView xWindow="20000" yWindow="460" windowWidth="26440" windowHeight="15440" activeTab="1" xr2:uid="{97C33AB7-0840-E244-BC44-7C9BE2576C51}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="MetaData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Node</t>
   </si>
@@ -56,15 +57,54 @@
   <si>
     <t>c</t>
   </si>
+  <si>
+    <t>MetaData</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Node: The clusters with identifiers 0-2499 that are involved in the solution for that trial.</t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t>c: the column of that cluster, for plotting (0-49)</t>
+  </si>
+  <si>
+    <t>r: the row of that cluster, for plotting (0,49)</t>
+  </si>
+  <si>
+    <t>f#: The frequency of nodes for a trial # (1,2,3,4 correspond to 1,2,2+,2-)</t>
+  </si>
+  <si>
+    <t>fall: sum of frequencies of nodes over all 4 models</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -86,15 +126,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -134,10 +211,10 @@
     <tableColumn id="6" xr3:uid="{025B590F-E115-B94C-91AC-BFD5178DBC44}" name="fall" dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[f1]:[f4]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{711D2B08-96A8-F54A-9966-085703347B2E}" name="r" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{711D2B08-96A8-F54A-9966-085703347B2E}" name="r" dataDxfId="1">
       <calculatedColumnFormula>MOD(Table1[[#This Row],[Node]],50)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{79ABCA47-C888-4B40-ACF4-5B8CF5711270}" name="c" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{79ABCA47-C888-4B40-ACF4-5B8CF5711270}" name="c" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.FLOOR.MATH(Table1[[#This Row],[Node]]/50)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -444,13 +521,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0838A6-91C6-0F41-9212-C05DAD77D8B2}">
   <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>27</v>
       </c>
@@ -505,7 +582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>80</v>
       </c>
@@ -534,7 +611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>329</v>
       </c>
@@ -563,7 +640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>378</v>
       </c>
@@ -592,7 +669,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>417</v>
       </c>
@@ -621,7 +698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>467</v>
       </c>
@@ -650,7 +727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>525</v>
       </c>
@@ -679,7 +756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>560</v>
       </c>
@@ -708,7 +785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>567</v>
       </c>
@@ -737,7 +814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>617</v>
       </c>
@@ -766,7 +843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>667</v>
       </c>
@@ -795,7 +872,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>706</v>
       </c>
@@ -824,7 +901,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>717</v>
       </c>
@@ -853,7 +930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>718</v>
       </c>
@@ -882,7 +959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>750</v>
       </c>
@@ -911,7 +988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>756</v>
       </c>
@@ -940,7 +1017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>775</v>
       </c>
@@ -969,7 +1046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>803</v>
       </c>
@@ -998,7 +1075,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>805</v>
       </c>
@@ -1027,7 +1104,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>852</v>
       </c>
@@ -1056,7 +1133,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>853</v>
       </c>
@@ -1085,7 +1162,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>854</v>
       </c>
@@ -1114,7 +1191,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>903</v>
       </c>
@@ -1143,7 +1220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>904</v>
       </c>
@@ -1172,7 +1249,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>951</v>
       </c>
@@ -1201,7 +1278,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>952</v>
       </c>
@@ -1230,7 +1307,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>1008</v>
       </c>
@@ -1259,7 +1336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>1013</v>
       </c>
@@ -1288,7 +1365,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>1020</v>
       </c>
@@ -1317,7 +1394,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>1021</v>
       </c>
@@ -1346,7 +1423,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>1022</v>
       </c>
@@ -1375,7 +1452,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>1037</v>
       </c>
@@ -1404,7 +1481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>1062</v>
       </c>
@@ -1433,7 +1510,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>1063</v>
       </c>
@@ -1462,7 +1539,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>1071</v>
       </c>
@@ -1491,7 +1568,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>1072</v>
       </c>
@@ -1520,7 +1597,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>1084</v>
       </c>
@@ -1549,7 +1626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>1087</v>
       </c>
@@ -1578,7 +1655,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>1088</v>
       </c>
@@ -1607,7 +1684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>1101</v>
       </c>
@@ -1636,7 +1713,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>1123</v>
       </c>
@@ -1665,7 +1742,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>1130</v>
       </c>
@@ -1694,7 +1771,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>1137</v>
       </c>
@@ -1723,7 +1800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>1138</v>
       </c>
@@ -1752,7 +1829,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>1139</v>
       </c>
@@ -1781,7 +1858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>1142</v>
       </c>
@@ -1810,7 +1887,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>1145</v>
       </c>
@@ -1839,7 +1916,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8">
       <c r="A49">
         <v>1151</v>
       </c>
@@ -1868,7 +1945,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8">
       <c r="A50">
         <v>1152</v>
       </c>
@@ -1897,7 +1974,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>1187</v>
       </c>
@@ -1926,7 +2003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8">
       <c r="A52">
         <v>1194</v>
       </c>
@@ -1955,7 +2032,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8">
       <c r="A53">
         <v>1200</v>
       </c>
@@ -1984,7 +2061,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8">
       <c r="A54">
         <v>1201</v>
       </c>
@@ -2013,7 +2090,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8">
       <c r="A55">
         <v>1202</v>
       </c>
@@ -2042,7 +2119,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8">
       <c r="A56">
         <v>1208</v>
       </c>
@@ -2071,7 +2148,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8">
       <c r="A57">
         <v>1214</v>
       </c>
@@ -2100,7 +2177,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8">
       <c r="A58">
         <v>1250</v>
       </c>
@@ -2129,7 +2206,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8">
       <c r="A59">
         <v>1251</v>
       </c>
@@ -2158,7 +2235,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8">
       <c r="A60">
         <v>1252</v>
       </c>
@@ -2187,7 +2264,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8">
       <c r="A61">
         <v>1257</v>
       </c>
@@ -2216,7 +2293,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8">
       <c r="A62">
         <v>1268</v>
       </c>
@@ -2245,7 +2322,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8">
       <c r="A63">
         <v>1290</v>
       </c>
@@ -2274,7 +2351,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8">
       <c r="A64">
         <v>1298</v>
       </c>
@@ -2303,7 +2380,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8">
       <c r="A65">
         <v>1299</v>
       </c>
@@ -2332,7 +2409,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8">
       <c r="A66">
         <v>1300</v>
       </c>
@@ -2361,7 +2438,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8">
       <c r="A67">
         <v>1302</v>
       </c>
@@ -2390,7 +2467,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8">
       <c r="A68">
         <v>1303</v>
       </c>
@@ -2419,7 +2496,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8">
       <c r="A69">
         <v>1318</v>
       </c>
@@ -2448,7 +2525,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8">
       <c r="A70">
         <v>1347</v>
       </c>
@@ -2477,7 +2554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8">
       <c r="A71">
         <v>1348</v>
       </c>
@@ -2506,7 +2583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8">
       <c r="A72">
         <v>1351</v>
       </c>
@@ -2535,7 +2612,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8">
       <c r="A73">
         <v>1353</v>
       </c>
@@ -2564,7 +2641,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8">
       <c r="A74">
         <v>1354</v>
       </c>
@@ -2593,7 +2670,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8">
       <c r="A75">
         <v>1367</v>
       </c>
@@ -2622,7 +2699,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8">
       <c r="A76">
         <v>1390</v>
       </c>
@@ -2651,7 +2728,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8">
       <c r="A77">
         <v>1397</v>
       </c>
@@ -2680,7 +2757,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8">
       <c r="A78">
         <v>1398</v>
       </c>
@@ -2709,7 +2786,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8">
       <c r="A79">
         <v>1437</v>
       </c>
@@ -2738,7 +2815,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8">
       <c r="A80">
         <v>1443</v>
       </c>
@@ -2767,7 +2844,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8">
       <c r="A81">
         <v>1444</v>
       </c>
@@ -2796,7 +2873,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8">
       <c r="A82">
         <v>1445</v>
       </c>
@@ -2825,7 +2902,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8">
       <c r="A83">
         <v>1446</v>
       </c>
@@ -2854,7 +2931,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8">
       <c r="A84">
         <v>1447</v>
       </c>
@@ -2883,7 +2960,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8">
       <c r="A85">
         <v>1448</v>
       </c>
@@ -2912,7 +2989,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8">
       <c r="A86">
         <v>1453</v>
       </c>
@@ -2941,7 +3018,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8">
       <c r="A87">
         <v>1470</v>
       </c>
@@ -2970,7 +3047,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8">
       <c r="A88">
         <v>1482</v>
       </c>
@@ -2999,7 +3076,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8">
       <c r="A89">
         <v>1486</v>
       </c>
@@ -3028,7 +3105,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8">
       <c r="A90">
         <v>1487</v>
       </c>
@@ -3057,7 +3134,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8">
       <c r="A91">
         <v>1488</v>
       </c>
@@ -3086,7 +3163,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8">
       <c r="A92">
         <v>1492</v>
       </c>
@@ -3115,7 +3192,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8">
       <c r="A93">
         <v>1493</v>
       </c>
@@ -3144,7 +3221,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8">
       <c r="A94">
         <v>1494</v>
       </c>
@@ -3173,7 +3250,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8">
       <c r="A95">
         <v>1496</v>
       </c>
@@ -3202,7 +3279,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8">
       <c r="A96">
         <v>1514</v>
       </c>
@@ -3231,7 +3308,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8">
       <c r="A97">
         <v>1538</v>
       </c>
@@ -3260,7 +3337,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8">
       <c r="A98">
         <v>1540</v>
       </c>
@@ -3289,7 +3366,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8">
       <c r="A99">
         <v>1541</v>
       </c>
@@ -3318,7 +3395,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8">
       <c r="A100">
         <v>1542</v>
       </c>
@@ -3347,7 +3424,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8">
       <c r="A101">
         <v>1545</v>
       </c>
@@ -3376,7 +3453,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8">
       <c r="A102">
         <v>1570</v>
       </c>
@@ -3405,7 +3482,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8">
       <c r="A103">
         <v>1587</v>
       </c>
@@ -3434,7 +3511,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8">
       <c r="A104">
         <v>1591</v>
       </c>
@@ -3463,7 +3540,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8">
       <c r="A105">
         <v>1592</v>
       </c>
@@ -3492,7 +3569,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8">
       <c r="A106">
         <v>1593</v>
       </c>
@@ -3521,7 +3598,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8">
       <c r="A107">
         <v>1638</v>
       </c>
@@ -3550,7 +3627,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8">
       <c r="A108">
         <v>1640</v>
       </c>
@@ -3579,7 +3656,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8">
       <c r="A109">
         <v>1641</v>
       </c>
@@ -3608,7 +3685,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8">
       <c r="A110">
         <v>1642</v>
       </c>
@@ -3637,7 +3714,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8">
       <c r="A111">
         <v>1643</v>
       </c>
@@ -3666,7 +3743,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8">
       <c r="A112">
         <v>1644</v>
       </c>
@@ -3695,7 +3772,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8">
       <c r="A113">
         <v>1675</v>
       </c>
@@ -3724,7 +3801,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8">
       <c r="A114">
         <v>1676</v>
       </c>
@@ -3753,7 +3830,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8">
       <c r="A115">
         <v>1682</v>
       </c>
@@ -3782,7 +3859,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8">
       <c r="A116">
         <v>1687</v>
       </c>
@@ -3811,7 +3888,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8">
       <c r="A117">
         <v>1688</v>
       </c>
@@ -3840,7 +3917,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8">
       <c r="A118">
         <v>1690</v>
       </c>
@@ -3869,7 +3946,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8">
       <c r="A119">
         <v>1691</v>
       </c>
@@ -3898,7 +3975,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8">
       <c r="A120">
         <v>1692</v>
       </c>
@@ -3927,7 +4004,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8">
       <c r="A121">
         <v>1693</v>
       </c>
@@ -3956,7 +4033,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8">
       <c r="A122">
         <v>1725</v>
       </c>
@@ -3985,7 +4062,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8">
       <c r="A123">
         <v>1726</v>
       </c>
@@ -4014,7 +4091,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8">
       <c r="A124">
         <v>1728</v>
       </c>
@@ -4043,7 +4120,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8">
       <c r="A125">
         <v>1730</v>
       </c>
@@ -4072,7 +4149,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8">
       <c r="A126">
         <v>1734</v>
       </c>
@@ -4101,7 +4178,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8">
       <c r="A127">
         <v>1735</v>
       </c>
@@ -4130,7 +4207,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8">
       <c r="A128">
         <v>1739</v>
       </c>
@@ -4159,7 +4236,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8">
       <c r="A129">
         <v>1740</v>
       </c>
@@ -4188,7 +4265,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8">
       <c r="A130">
         <v>1741</v>
       </c>
@@ -4217,7 +4294,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8">
       <c r="A131">
         <v>1743</v>
       </c>
@@ -4246,7 +4323,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8">
       <c r="A132">
         <v>1782</v>
       </c>
@@ -4275,7 +4352,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8">
       <c r="A133">
         <v>1784</v>
       </c>
@@ -4304,7 +4381,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8">
       <c r="A134">
         <v>1785</v>
       </c>
@@ -4333,7 +4410,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8">
       <c r="A135">
         <v>1789</v>
       </c>
@@ -4362,7 +4439,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8">
       <c r="A136">
         <v>1791</v>
       </c>
@@ -4391,7 +4468,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8">
       <c r="A137">
         <v>1815</v>
       </c>
@@ -4420,7 +4497,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8">
       <c r="A138">
         <v>1816</v>
       </c>
@@ -4449,7 +4526,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8">
       <c r="A139">
         <v>1837</v>
       </c>
@@ -4478,7 +4555,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8">
       <c r="A140">
         <v>1838</v>
       </c>
@@ -4507,7 +4584,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8">
       <c r="A141">
         <v>1936</v>
       </c>
@@ -4536,7 +4613,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8">
       <c r="A142">
         <v>1968</v>
       </c>
@@ -4565,7 +4642,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8">
       <c r="A143">
         <v>1985</v>
       </c>
@@ -4594,7 +4671,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8">
       <c r="A144">
         <v>2013</v>
       </c>
@@ -4623,7 +4700,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8">
       <c r="A145">
         <v>2027</v>
       </c>
@@ -4652,7 +4729,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8">
       <c r="A146">
         <v>2036</v>
       </c>
@@ -4681,7 +4758,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8">
       <c r="A147">
         <v>2072</v>
       </c>
@@ -4710,7 +4787,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8">
       <c r="A148">
         <v>2076</v>
       </c>
@@ -4739,7 +4816,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8">
       <c r="A149">
         <v>2084</v>
       </c>
@@ -4768,7 +4845,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8">
       <c r="A150">
         <v>2175</v>
       </c>
@@ -4797,7 +4874,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8">
       <c r="A151">
         <v>2176</v>
       </c>
@@ -4826,7 +4903,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8">
       <c r="A152">
         <v>2232</v>
       </c>
@@ -4855,7 +4932,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8">
       <c r="A153">
         <v>2281</v>
       </c>
@@ -4884,7 +4961,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8">
       <c r="A154">
         <v>2431</v>
       </c>
@@ -4913,7 +4990,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8">
       <c r="A155">
         <v>2478</v>
       </c>
@@ -4942,7 +5019,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8">
       <c r="A156">
         <v>2481</v>
       </c>
@@ -4977,4 +5054,93 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE7508F-740F-694B-8D2C-E45953DFE538}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" ht="32" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="21" thickBot="1">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="34" customHeight="1" thickTop="1">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="21" thickBot="1">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="17" thickTop="1">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>